<commit_message>
GreatestConsecutivePositiveNumbers and Vowels and Consonants
</commit_message>
<xml_diff>
--- a/SortingTechniques.xlsx
+++ b/SortingTechniques.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashwin_Gudepu\Documents\AshwinAssignments\trainingandmentoring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\practicePrograms\FrameworkStructure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA737C7F-5EDD-4BCB-AD27-6B93B47C1995}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="7" xr2:uid="{547E1945-37E8-4D52-BC1A-1C0313917545}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BubbleSort" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
     <sheet name="Permutations" sheetId="12" r:id="rId8"/>
     <sheet name="Sheet2" sheetId="13" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="141">
   <si>
     <t>Bubble Sort</t>
   </si>
@@ -806,11 +805,177 @@
   <si>
     <t>4-&gt;4*3*2*1=24</t>
   </si>
+  <si>
+    <t>Every time we take Temp and compare with the sorted set, if temp is 
+less than the sorted values then swapping will be done</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">if(last element &gt; Pivot element)   { move the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>END</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">}
+else  {stop </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>END</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">if( First element&lt;= Pivot element)   { move the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>START</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">}
+else  {stop </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>START</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Swap </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>START</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>END</t>
+    </r>
+  </si>
+  <si>
+    <t>Step 1</t>
+  </si>
+  <si>
+    <t>Step 2</t>
+  </si>
+  <si>
+    <t>Step 3</t>
+  </si>
+  <si>
+    <t>Step 4</t>
+  </si>
+  <si>
+    <t>If START crossess END then swap Pivot element with START element.
+After this Pivot element will change and will get the
+exact position.
+ All the elements towards Leftside of the Pivot
+element are less than the Pivot Element and all the Elements towards Right side are greater then Pivot elements</t>
+  </si>
+  <si>
+    <t>for(int i=1;i&lt;n;i++){
+      int j=i-1;
+       while(j&gt;=0 &amp;&amp; a[j]&gt;temp){
+            a[j+1]=a[i];
+             j--;
+         }
+  a[j+1] =temp;
+}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -966,7 +1131,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="50">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -1601,11 +1766,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="224">
+  <cellXfs count="258">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2166,6 +2355,42 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2184,41 +2409,105 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2533,20 +2822,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{547E7C85-E0A7-42EA-B069-25A1F1A29B8B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3:N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.1796875" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="146" t="s">
         <v>2</v>
       </c>
@@ -2556,7 +2845,7 @@
       <c r="F2" s="147"/>
       <c r="G2" s="148"/>
     </row>
-    <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="155" t="s">
         <v>0</v>
       </c>
@@ -2575,7 +2864,7 @@
       <c r="M3" s="145"/>
       <c r="N3" s="145"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
@@ -2599,7 +2888,7 @@
       <c r="M4" s="145"/>
       <c r="N4" s="145"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="153" t="s">
         <v>7</v>
       </c>
@@ -2617,7 +2906,7 @@
       <c r="M5" s="145"/>
       <c r="N5" s="145"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="153"/>
       <c r="C6" s="17"/>
       <c r="D6" s="1">
@@ -2633,7 +2922,7 @@
       <c r="M6" s="145"/>
       <c r="N6" s="145"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="153"/>
       <c r="C7" s="18"/>
       <c r="D7" s="17"/>
@@ -2649,7 +2938,7 @@
       <c r="M7" s="145"/>
       <c r="N7" s="145"/>
     </row>
-    <row r="8" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="154"/>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -2665,7 +2954,7 @@
       <c r="M8" s="145"/>
       <c r="N8" s="145"/>
     </row>
-    <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="13" t="s">
         <v>1</v>
       </c>
@@ -2689,7 +2978,7 @@
       <c r="M9" s="145"/>
       <c r="N9" s="145"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="149" t="s">
         <v>8</v>
       </c>
@@ -2713,7 +3002,7 @@
       <c r="M10" s="145"/>
       <c r="N10" s="145"/>
     </row>
-    <row r="11" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="150"/>
       <c r="C11" s="5">
         <v>6</v>
@@ -2725,7 +3014,7 @@
       <c r="F11" s="5"/>
       <c r="G11" s="12"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="150"/>
       <c r="C12" s="1"/>
       <c r="D12" s="6">
@@ -2737,7 +3026,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="150"/>
       <c r="C13" s="1"/>
       <c r="D13" s="6"/>
@@ -2749,7 +3038,7 @@
       </c>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="151"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2761,7 +3050,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="14" t="s">
         <v>3</v>
       </c>
@@ -2781,7 +3070,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="152" t="s">
         <v>9</v>
       </c>
@@ -2801,7 +3090,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="150"/>
       <c r="C17" s="5">
         <v>6</v>
@@ -2813,7 +3102,7 @@
       <c r="F17" s="5"/>
       <c r="G17" s="12"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="150"/>
       <c r="C18" s="1"/>
       <c r="D18" s="6">
@@ -2825,7 +3114,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="150"/>
       <c r="C19" s="1"/>
       <c r="D19" s="6"/>
@@ -2837,7 +3126,7 @@
       </c>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="151"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2849,7 +3138,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="14" t="s">
         <v>4</v>
       </c>
@@ -2869,7 +3158,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="152" t="s">
         <v>10</v>
       </c>
@@ -2889,7 +3178,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="150"/>
       <c r="C23" s="5">
         <v>5</v>
@@ -2901,7 +3190,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="12"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="150"/>
       <c r="C24" s="1"/>
       <c r="D24" s="6">
@@ -2913,7 +3202,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="150"/>
       <c r="C25" s="1"/>
       <c r="D25" s="6"/>
@@ -2925,7 +3214,7 @@
       </c>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="151"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -2937,7 +3226,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="14" t="s">
         <v>5</v>
       </c>
@@ -2973,22 +3262,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7483B630-F6BC-4188-A3FE-E8BFEB5BDA7A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:L12"/>
   <sheetViews>
     <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="D7" sqref="D7:I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.36328125" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C2" s="36" t="s">
         <v>11</v>
       </c>
@@ -3001,7 +3290,7 @@
       <c r="H2" s="29"/>
       <c r="I2" s="29"/>
     </row>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C3" s="38" t="s">
         <v>12</v>
       </c>
@@ -3009,7 +3298,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="39" t="s">
         <v>13</v>
       </c>
@@ -3017,13 +3306,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K5" s="161" t="s">
         <v>16</v>
       </c>
       <c r="L5" s="162"/>
     </row>
-    <row r="6" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="163" t="s">
         <v>21</v>
       </c>
@@ -3037,7 +3326,7 @@
       </c>
       <c r="L6" s="32"/>
     </row>
-    <row r="7" spans="3:12" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="3:12" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="158" t="s">
         <v>77</v>
       </c>
@@ -3047,7 +3336,7 @@
       <c r="H7" s="159"/>
       <c r="I7" s="160"/>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C8" s="33" t="s">
         <v>14</v>
       </c>
@@ -3070,7 +3359,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C9" s="33" t="s">
         <v>17</v>
       </c>
@@ -3093,7 +3382,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C10" s="33" t="s">
         <v>18</v>
       </c>
@@ -3116,7 +3405,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C11" s="33" t="s">
         <v>19</v>
       </c>
@@ -3139,7 +3428,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C12" s="33" t="s">
         <v>20</v>
       </c>
@@ -3174,22 +3463,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B48F29-5F28-40E5-8536-B655C419E2EC}">
-  <dimension ref="B1:N31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:T31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3:T10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.08984375" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="36" t="s">
         <v>11</v>
       </c>
@@ -3197,29 +3486,54 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:20" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="38" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I3" s="144" t="s">
+        <v>131</v>
+      </c>
+      <c r="J3" s="145"/>
+      <c r="K3" s="145"/>
+      <c r="L3" s="145"/>
+      <c r="M3" s="145"/>
+      <c r="N3" s="145"/>
+      <c r="P3" s="250" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q3" s="251"/>
+      <c r="R3" s="251"/>
+      <c r="S3" s="251"/>
+      <c r="T3" s="252"/>
+    </row>
+    <row r="4" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="39" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="41" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P4" s="253"/>
+      <c r="Q4" s="249"/>
+      <c r="R4" s="249"/>
+      <c r="S4" s="249"/>
+      <c r="T4" s="254"/>
+    </row>
+    <row r="5" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I5" s="168" t="s">
         <v>26</v>
       </c>
       <c r="J5" s="168"/>
-    </row>
-    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P5" s="253"/>
+      <c r="Q5" s="249"/>
+      <c r="R5" s="249"/>
+      <c r="S5" s="249"/>
+      <c r="T5" s="254"/>
+    </row>
+    <row r="6" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="163" t="s">
         <v>24</v>
       </c>
@@ -3232,8 +3546,13 @@
         <v>16</v>
       </c>
       <c r="J6" s="162"/>
-    </row>
-    <row r="7" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P6" s="253"/>
+      <c r="Q6" s="249"/>
+      <c r="R6" s="249"/>
+      <c r="S6" s="249"/>
+      <c r="T6" s="254"/>
+    </row>
+    <row r="7" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="158" t="s">
         <v>22</v>
       </c>
@@ -3246,9 +3565,20 @@
         <v>15</v>
       </c>
       <c r="J7" s="32"/>
-    </row>
-    <row r="8" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="P7" s="253"/>
+      <c r="Q7" s="249"/>
+      <c r="R7" s="249"/>
+      <c r="S7" s="249"/>
+      <c r="T7" s="254"/>
+    </row>
+    <row r="8" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P8" s="253"/>
+      <c r="Q8" s="249"/>
+      <c r="R8" s="249"/>
+      <c r="S8" s="249"/>
+      <c r="T8" s="254"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C9" s="45">
         <v>5</v>
       </c>
@@ -3270,8 +3600,13 @@
       <c r="J9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P9" s="253"/>
+      <c r="Q9" s="249"/>
+      <c r="R9" s="249"/>
+      <c r="S9" s="249"/>
+      <c r="T9" s="254"/>
+    </row>
+    <row r="10" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="50">
         <v>4</v>
       </c>
@@ -3290,8 +3625,13 @@
       <c r="H10" s="52">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P10" s="255"/>
+      <c r="Q10" s="256"/>
+      <c r="R10" s="256"/>
+      <c r="S10" s="256"/>
+      <c r="T10" s="257"/>
+    </row>
+    <row r="11" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="44"/>
       <c r="D11" s="44"/>
       <c r="E11" s="44"/>
@@ -3299,7 +3639,7 @@
       <c r="G11" s="44"/>
       <c r="H11" s="44"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C12" s="45">
         <v>4</v>
       </c>
@@ -3322,7 +3662,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="2:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="50">
         <v>4</v>
       </c>
@@ -3349,7 +3689,7 @@
       <c r="M13" s="145"/>
       <c r="N13" s="145"/>
     </row>
-    <row r="14" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="44"/>
       <c r="D14" s="44"/>
       <c r="E14" s="44"/>
@@ -3357,7 +3697,7 @@
       <c r="G14" s="44"/>
       <c r="H14" s="44"/>
     </row>
-    <row r="15" spans="2:14" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:20" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="45">
         <v>4</v>
       </c>
@@ -3384,7 +3724,7 @@
       <c r="M15" s="145"/>
       <c r="N15" s="145"/>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C16" s="53">
         <v>4</v>
       </c>
@@ -3407,7 +3747,7 @@
       <c r="M16" s="145"/>
       <c r="N16" s="145"/>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C17" s="53">
         <v>4</v>
       </c>
@@ -3425,7 +3765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C18" s="53"/>
       <c r="D18" s="54">
         <v>4</v>
@@ -3443,7 +3783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="3:14" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="50">
         <v>1</v>
       </c>
@@ -3470,7 +3810,7 @@
       <c r="M19" s="167"/>
       <c r="N19" s="167"/>
     </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C20" s="44"/>
       <c r="D20" s="44"/>
       <c r="E20" s="44"/>
@@ -3478,7 +3818,7 @@
       <c r="G20" s="44"/>
       <c r="H20" s="44"/>
     </row>
-    <row r="21" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="44"/>
       <c r="D21" s="44"/>
       <c r="E21" s="44"/>
@@ -3486,7 +3826,7 @@
       <c r="G21" s="44"/>
       <c r="H21" s="44"/>
     </row>
-    <row r="22" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="59">
         <v>1</v>
       </c>
@@ -3509,7 +3849,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="50">
         <v>1</v>
       </c>
@@ -3527,7 +3867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="50">
         <v>1</v>
       </c>
@@ -3547,8 +3887,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C26" s="45">
         <v>1</v>
       </c>
@@ -3568,7 +3908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C27" s="53">
         <v>1</v>
       </c>
@@ -3586,7 +3926,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C28" s="53">
         <v>1</v>
       </c>
@@ -3604,7 +3944,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C29" s="53">
         <v>1</v>
       </c>
@@ -3622,7 +3962,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C30" s="53">
         <v>1</v>
       </c>
@@ -3640,7 +3980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="50">
         <v>1</v>
       </c>
@@ -3661,7 +4001,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="I3:N3"/>
+    <mergeCell ref="P3:T10"/>
     <mergeCell ref="J19:N19"/>
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="B7:G7"/>
@@ -3675,34 +4017,40 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6817E4F7-28A1-4CBF-B79A-00F49139067C}">
-  <dimension ref="B1:N43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:V43"/>
   <sheetViews>
     <sheetView zoomScale="97" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:F18"/>
+      <selection activeCell="Q5" sqref="Q5:Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.1796875" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="3:22" x14ac:dyDescent="0.25">
       <c r="F2" s="172" t="s">
         <v>66</v>
       </c>
       <c r="G2" s="173"/>
     </row>
-    <row r="3" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F3" s="170" t="s">
         <v>69</v>
       </c>
       <c r="G3" s="171"/>
     </row>
-    <row r="4" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P4" s="224"/>
+      <c r="Q4" s="225"/>
+      <c r="R4" s="225"/>
+      <c r="S4" s="225"/>
+      <c r="T4" s="225"/>
+    </row>
+    <row r="5" spans="3:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="174" t="s">
         <v>72</v>
       </c>
@@ -3733,8 +4081,19 @@
       <c r="L5" s="70">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="P5" s="224"/>
+      <c r="Q5" s="227" t="s">
+        <v>135</v>
+      </c>
+      <c r="R5" s="228" t="s">
+        <v>133</v>
+      </c>
+      <c r="S5" s="228"/>
+      <c r="T5" s="228"/>
+      <c r="U5" s="228"/>
+      <c r="V5" s="229"/>
+    </row>
+    <row r="6" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="175"/>
       <c r="D6" s="116" t="s">
         <v>65</v>
@@ -3751,8 +4110,15 @@
       <c r="L6" s="108" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="P6" s="224"/>
+      <c r="Q6" s="230"/>
+      <c r="R6" s="231"/>
+      <c r="S6" s="231"/>
+      <c r="T6" s="231"/>
+      <c r="U6" s="231"/>
+      <c r="V6" s="232"/>
+    </row>
+    <row r="7" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="175"/>
       <c r="D7" s="116">
         <v>34</v>
@@ -3781,8 +4147,15 @@
       <c r="L7" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="P7" s="225"/>
+      <c r="Q7" s="226"/>
+      <c r="R7" s="225"/>
+      <c r="S7" s="225"/>
+      <c r="T7" s="225"/>
+      <c r="U7" s="225"/>
+      <c r="V7" s="225"/>
+    </row>
+    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C8" s="175"/>
       <c r="D8" s="116" t="s">
         <v>65</v>
@@ -3799,8 +4172,19 @@
         <v>70</v>
       </c>
       <c r="L8" s="108"/>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="P8" s="225"/>
+      <c r="Q8" s="227" t="s">
+        <v>136</v>
+      </c>
+      <c r="R8" s="228" t="s">
+        <v>132</v>
+      </c>
+      <c r="S8" s="228"/>
+      <c r="T8" s="228"/>
+      <c r="U8" s="228"/>
+      <c r="V8" s="229"/>
+    </row>
+    <row r="9" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="175"/>
       <c r="D9" s="116">
         <v>34</v>
@@ -3829,8 +4213,15 @@
       <c r="L9" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="P9" s="225"/>
+      <c r="Q9" s="230"/>
+      <c r="R9" s="231"/>
+      <c r="S9" s="231"/>
+      <c r="T9" s="231"/>
+      <c r="U9" s="231"/>
+      <c r="V9" s="232"/>
+    </row>
+    <row r="10" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="175"/>
       <c r="D10" s="116" t="s">
         <v>65</v>
@@ -3847,8 +4238,13 @@
       <c r="J10" s="33"/>
       <c r="K10" s="33"/>
       <c r="L10" s="108"/>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="P10" s="225"/>
+      <c r="Q10" s="226"/>
+      <c r="R10" s="225"/>
+      <c r="S10" s="225"/>
+      <c r="T10" s="225"/>
+    </row>
+    <row r="11" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C11" s="175"/>
       <c r="D11" s="116">
         <v>34</v>
@@ -3877,8 +4273,19 @@
       <c r="L11" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="P11" s="225"/>
+      <c r="Q11" s="227" t="s">
+        <v>137</v>
+      </c>
+      <c r="R11" s="233" t="s">
+        <v>134</v>
+      </c>
+      <c r="S11" s="233"/>
+      <c r="T11" s="233"/>
+      <c r="U11" s="233"/>
+      <c r="V11" s="234"/>
+    </row>
+    <row r="12" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="175"/>
       <c r="D12" s="116" t="s">
         <v>65</v>
@@ -3895,8 +4302,15 @@
       <c r="J12" s="33"/>
       <c r="K12" s="33"/>
       <c r="L12" s="108"/>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="P12" s="225"/>
+      <c r="Q12" s="230"/>
+      <c r="R12" s="235"/>
+      <c r="S12" s="235"/>
+      <c r="T12" s="235"/>
+      <c r="U12" s="235"/>
+      <c r="V12" s="236"/>
+    </row>
+    <row r="13" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="175"/>
       <c r="D13" s="117">
         <v>9</v>
@@ -3925,8 +4339,13 @@
       <c r="L13" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P13" s="225"/>
+      <c r="Q13" s="226"/>
+      <c r="R13" s="225"/>
+      <c r="S13" s="225"/>
+      <c r="T13" s="225"/>
+    </row>
+    <row r="14" spans="3:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="170"/>
       <c r="D14" s="127" t="s">
         <v>65</v>
@@ -3943,8 +4362,37 @@
       <c r="J14" s="109"/>
       <c r="K14" s="109"/>
       <c r="L14" s="40"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="P14" s="225"/>
+      <c r="Q14" s="237" t="s">
+        <v>138</v>
+      </c>
+      <c r="R14" s="242" t="s">
+        <v>139</v>
+      </c>
+      <c r="S14" s="240"/>
+      <c r="T14" s="240"/>
+      <c r="U14" s="240"/>
+      <c r="V14" s="243"/>
+    </row>
+    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="P15" s="225"/>
+      <c r="Q15" s="238"/>
+      <c r="R15" s="244"/>
+      <c r="S15" s="241"/>
+      <c r="T15" s="241"/>
+      <c r="U15" s="241"/>
+      <c r="V15" s="245"/>
+    </row>
+    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="P16" s="225"/>
+      <c r="Q16" s="238"/>
+      <c r="R16" s="244"/>
+      <c r="S16" s="241"/>
+      <c r="T16" s="241"/>
+      <c r="U16" s="241"/>
+      <c r="V16" s="245"/>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D17" s="118">
         <v>9</v>
       </c>
@@ -3972,8 +4420,15 @@
       <c r="L17" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="P17" s="225"/>
+      <c r="Q17" s="238"/>
+      <c r="R17" s="244"/>
+      <c r="S17" s="241"/>
+      <c r="T17" s="241"/>
+      <c r="U17" s="241"/>
+      <c r="V17" s="245"/>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D18" s="118" t="s">
         <v>65</v>
       </c>
@@ -3985,8 +4440,24 @@
       <c r="J18" s="33"/>
       <c r="K18" s="33"/>
       <c r="L18" s="33"/>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="P18" s="225"/>
+      <c r="Q18" s="238"/>
+      <c r="R18" s="244"/>
+      <c r="S18" s="241"/>
+      <c r="T18" s="241"/>
+      <c r="U18" s="241"/>
+      <c r="V18" s="245"/>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="P19" s="225"/>
+      <c r="Q19" s="238"/>
+      <c r="R19" s="244"/>
+      <c r="S19" s="241"/>
+      <c r="T19" s="241"/>
+      <c r="U19" s="241"/>
+      <c r="V19" s="245"/>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B20" s="121"/>
       <c r="C20" s="121"/>
       <c r="D20" s="118">
@@ -4017,8 +4488,15 @@
         <v>73</v>
       </c>
       <c r="N20" s="176"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="P20" s="225"/>
+      <c r="Q20" s="238"/>
+      <c r="R20" s="244"/>
+      <c r="S20" s="241"/>
+      <c r="T20" s="241"/>
+      <c r="U20" s="241"/>
+      <c r="V20" s="245"/>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B21" s="107"/>
       <c r="C21" s="107"/>
       <c r="D21" s="120" t="s">
@@ -4043,8 +4521,14 @@
       </c>
       <c r="M21" s="176"/>
       <c r="N21" s="176"/>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="Q21" s="238"/>
+      <c r="R21" s="244"/>
+      <c r="S21" s="241"/>
+      <c r="T21" s="241"/>
+      <c r="U21" s="241"/>
+      <c r="V21" s="245"/>
+    </row>
+    <row r="22" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H22" s="33"/>
       <c r="I22" s="33"/>
       <c r="J22" s="33"/>
@@ -4052,8 +4536,14 @@
       <c r="L22" s="33"/>
       <c r="M22" s="176"/>
       <c r="N22" s="176"/>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="Q22" s="239"/>
+      <c r="R22" s="246"/>
+      <c r="S22" s="247"/>
+      <c r="T22" s="247"/>
+      <c r="U22" s="247"/>
+      <c r="V22" s="248"/>
+    </row>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C23" s="169" t="s">
         <v>73</v>
       </c>
@@ -4084,7 +4574,7 @@
       <c r="M23" s="176"/>
       <c r="N23" s="176"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C24" s="169"/>
       <c r="D24" s="120" t="s">
         <v>65</v>
@@ -4109,7 +4599,7 @@
       <c r="M24" s="176"/>
       <c r="N24" s="176"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="J25" s="33"/>
@@ -4118,7 +4608,7 @@
       <c r="M25" s="176"/>
       <c r="N25" s="176"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C26" s="169" t="s">
         <v>73</v>
       </c>
@@ -4146,7 +4636,7 @@
       <c r="M26" s="176"/>
       <c r="N26" s="176"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C27" s="169"/>
       <c r="E27" s="122" t="s">
         <v>65</v>
@@ -4168,7 +4658,7 @@
       <c r="M27" s="176"/>
       <c r="N27" s="176"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
       <c r="H28" s="33"/>
       <c r="I28" s="33"/>
       <c r="J28" s="33"/>
@@ -4177,7 +4667,7 @@
       <c r="M28" s="176"/>
       <c r="N28" s="176"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D29">
         <v>9</v>
       </c>
@@ -4205,7 +4695,7 @@
       <c r="M29" s="176"/>
       <c r="N29" s="176"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
       <c r="H30" s="123" t="s">
         <v>65</v>
       </c>
@@ -4220,7 +4710,7 @@
       <c r="M30" s="176"/>
       <c r="N30" s="176"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
       <c r="H31" s="33"/>
       <c r="I31" s="33"/>
       <c r="J31" s="33"/>
@@ -4229,7 +4719,7 @@
       <c r="M31" s="176"/>
       <c r="N31" s="176"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
       <c r="H32" s="1">
         <v>40</v>
       </c>
@@ -4248,7 +4738,7 @@
       <c r="M32" s="176"/>
       <c r="N32" s="176"/>
     </row>
-    <row r="33" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:14" x14ac:dyDescent="0.25">
       <c r="H33" s="123" t="s">
         <v>65</v>
       </c>
@@ -4259,7 +4749,7 @@
       <c r="M33" s="176"/>
       <c r="N33" s="176"/>
     </row>
-    <row r="36" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:14" x14ac:dyDescent="0.25">
       <c r="H36" s="1">
         <v>40</v>
       </c>
@@ -4274,7 +4764,7 @@
       </c>
       <c r="N36" s="169"/>
     </row>
-    <row r="37" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:14" x14ac:dyDescent="0.25">
       <c r="H37" s="123" t="s">
         <v>65</v>
       </c>
@@ -4287,7 +4777,7 @@
       <c r="M37" s="169"/>
       <c r="N37" s="169"/>
     </row>
-    <row r="39" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:14" x14ac:dyDescent="0.25">
       <c r="I39" s="1">
         <v>60</v>
       </c>
@@ -4299,7 +4789,7 @@
       </c>
       <c r="N39" s="169"/>
     </row>
-    <row r="40" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:14" x14ac:dyDescent="0.25">
       <c r="I40" s="124" t="s">
         <v>65</v>
       </c>
@@ -4309,7 +4799,7 @@
       <c r="M40" s="169"/>
       <c r="N40" s="169"/>
     </row>
-    <row r="42" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D42" s="33">
         <v>9</v>
       </c>
@@ -4342,13 +4832,21 @@
       </c>
       <c r="N42" s="169"/>
     </row>
-    <row r="43" spans="4:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:14" x14ac:dyDescent="0.25">
       <c r="J43" s="125"/>
       <c r="M43" s="169"/>
       <c r="N43" s="169"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="17">
+    <mergeCell ref="R5:V6"/>
+    <mergeCell ref="R8:V9"/>
+    <mergeCell ref="R11:V12"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="R14:V22"/>
+    <mergeCell ref="Q14:Q22"/>
     <mergeCell ref="M39:N40"/>
     <mergeCell ref="M42:N43"/>
     <mergeCell ref="C23:C24"/>
@@ -4360,25 +4858,26 @@
     <mergeCell ref="M36:N37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6AB6F3-0B86-4D14-8F79-2B7D0DFFD564}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="6:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="6:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F2" s="177" t="s">
         <v>75</v>
       </c>
@@ -4386,7 +4885,7 @@
       <c r="H2" s="178"/>
       <c r="I2" s="179"/>
     </row>
-    <row r="3" spans="6:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="6:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F3" s="180" t="s">
         <v>74</v>
       </c>
@@ -4394,7 +4893,7 @@
       <c r="H3" s="159"/>
       <c r="I3" s="160"/>
     </row>
-    <row r="5" spans="6:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F5" s="118">
         <v>9</v>
       </c>
@@ -4408,7 +4907,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="6:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F6" s="118" t="s">
         <v>65</v>
       </c>
@@ -4419,7 +4918,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="6:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F8" s="118">
         <v>9</v>
       </c>
@@ -4430,7 +4929,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="6:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F9" s="118" t="s">
         <v>65</v>
       </c>
@@ -4451,26 +4950,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{223265B6-840B-4E22-ACFC-44A8315CD9B0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.36328125" customWidth="1"/>
-    <col min="10" max="10" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="30" t="s">
         <v>37</v>
       </c>
@@ -4484,7 +4983,7 @@
       <c r="K2" s="183"/>
       <c r="L2" s="184"/>
     </row>
-    <row r="3" spans="2:15" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:15" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F3" s="71" t="s">
         <v>38</v>
       </c>
@@ -4501,7 +5000,7 @@
       <c r="N3" s="186"/>
       <c r="O3" s="187"/>
     </row>
-    <row r="4" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F4" s="72" t="s">
         <v>39</v>
       </c>
@@ -4510,17 +5009,17 @@
       </c>
       <c r="H4" s="193"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F5" s="73"/>
       <c r="G5" s="74"/>
       <c r="H5" s="74"/>
     </row>
-    <row r="6" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F6" s="73"/>
       <c r="G6" s="74"/>
       <c r="H6" s="74"/>
     </row>
-    <row r="7" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="100"/>
       <c r="C7" s="101"/>
       <c r="D7" s="102"/>
@@ -4555,7 +5054,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="97" t="s">
         <v>34</v>
       </c>
@@ -4596,7 +5095,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="50">
         <v>0</v>
       </c>
@@ -4624,7 +5123,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F10" s="181" t="s">
         <v>47</v>
       </c>
@@ -4638,7 +5137,7 @@
       <c r="N10" s="181"/>
       <c r="O10" s="181"/>
     </row>
-    <row r="11" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="100"/>
       <c r="C11" s="101"/>
       <c r="D11" s="102"/>
@@ -4658,7 +5157,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="92" t="s">
         <v>34</v>
       </c>
@@ -4684,7 +5183,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="66">
         <v>5</v>
       </c>
@@ -4707,7 +5206,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F14" s="181" t="s">
         <v>48</v>
       </c>
@@ -4721,7 +5220,7 @@
       <c r="N14" s="181"/>
       <c r="O14" s="181"/>
     </row>
-    <row r="15" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="100"/>
       <c r="C15" s="101"/>
       <c r="D15" s="102"/>
@@ -4741,7 +5240,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="92" t="s">
         <v>34</v>
       </c>
@@ -4767,7 +5266,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="66">
         <v>5</v>
       </c>
@@ -4787,7 +5286,7 @@
       <c r="I17" s="41"/>
       <c r="J17" s="96"/>
     </row>
-    <row r="18" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="74"/>
       <c r="C18" s="74"/>
       <c r="D18" s="74"/>
@@ -4799,7 +5298,7 @@
       <c r="I18" s="74"/>
       <c r="J18" s="104"/>
     </row>
-    <row r="19" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="181" t="s">
         <v>49</v>
       </c>
@@ -4813,7 +5312,7 @@
       <c r="N19" s="181"/>
       <c r="O19" s="181"/>
     </row>
-    <row r="20" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="100"/>
       <c r="C20" s="101"/>
       <c r="D20" s="102"/>
@@ -4848,7 +5347,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="92" t="s">
         <v>34</v>
       </c>
@@ -4889,7 +5388,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="66">
         <v>6</v>
       </c>
@@ -4913,7 +5412,7 @@
       <c r="N22" s="41"/>
       <c r="O22" s="96"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
         <v>50</v>
       </c>
@@ -4934,21 +5433,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B9F5FD-7D98-404A-9D1E-C750930B0935}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E2:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="13.6328125" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="5:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E3" s="113"/>
       <c r="F3" s="64"/>
       <c r="G3" s="198" t="s">
@@ -4958,7 +5457,7 @@
       <c r="I3" s="198"/>
       <c r="J3" s="173"/>
     </row>
-    <row r="4" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E4" s="114"/>
       <c r="F4" s="6"/>
       <c r="G4" s="5" t="s">
@@ -4974,7 +5473,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E5" s="194" t="s">
         <v>58</v>
       </c>
@@ -4994,7 +5493,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E6" s="195"/>
       <c r="F6" s="110" t="s">
         <v>56</v>
@@ -5012,7 +5511,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E7" s="195"/>
       <c r="F7" s="110" t="s">
         <v>57</v>
@@ -5030,7 +5529,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="5:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="5:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E8" s="196" t="s">
         <v>59</v>
       </c>
@@ -5050,7 +5549,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="5:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E9" s="197"/>
       <c r="F9" s="112" t="s">
         <v>57</v>
@@ -5068,10 +5567,10 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E10" s="107"/>
     </row>
-    <row r="11" spans="5:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E11" s="145" t="s">
         <v>63</v>
       </c>
@@ -5094,25 +5593,25 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFE868DC-C44A-4B45-BFE9-F473441181CE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="37.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I3" s="135" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="136" t="s">
         <v>96</v>
       </c>
@@ -5134,7 +5633,7 @@
       <c r="M4" s="204"/>
       <c r="N4" s="202"/>
     </row>
-    <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="132"/>
       <c r="E5" s="137" t="s">
         <v>87</v>
@@ -5153,7 +5652,7 @@
       </c>
       <c r="N5" s="132"/>
     </row>
-    <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="136" t="s">
         <v>97</v>
       </c>
@@ -5175,7 +5674,7 @@
       <c r="M6" s="205"/>
       <c r="N6" s="204"/>
     </row>
-    <row r="7" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="129"/>
       <c r="D7" s="135" t="s">
         <v>87</v>
@@ -5201,12 +5700,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>130</v>
       </c>
@@ -5226,127 +5725,127 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C525961-E33A-4BB2-B350-8FD5B9FA2764}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AB7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="6.7265625" customWidth="1"/>
-    <col min="3" max="3" width="5.6328125" customWidth="1"/>
-    <col min="4" max="4" width="7.81640625" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" customWidth="1"/>
-    <col min="6" max="6" width="7.36328125" customWidth="1"/>
-    <col min="7" max="7" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="161" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="212"/>
-      <c r="D3" s="212"/>
-      <c r="E3" s="212"/>
-      <c r="F3" s="212"/>
-      <c r="G3" s="212"/>
-      <c r="H3" s="212"/>
-      <c r="I3" s="212"/>
-      <c r="J3" s="212"/>
-      <c r="K3" s="212"/>
-      <c r="L3" s="212"/>
-      <c r="M3" s="212"/>
-      <c r="N3" s="212"/>
-      <c r="O3" s="212"/>
-      <c r="P3" s="212"/>
-      <c r="Q3" s="212"/>
-      <c r="R3" s="212"/>
-      <c r="S3" s="212"/>
-      <c r="T3" s="212"/>
-      <c r="U3" s="212"/>
-      <c r="V3" s="212"/>
-      <c r="W3" s="212"/>
-      <c r="X3" s="212"/>
-      <c r="Y3" s="212"/>
-      <c r="Z3" s="212"/>
-      <c r="AA3" s="212"/>
+      <c r="C3" s="206"/>
+      <c r="D3" s="206"/>
+      <c r="E3" s="206"/>
+      <c r="F3" s="206"/>
+      <c r="G3" s="206"/>
+      <c r="H3" s="206"/>
+      <c r="I3" s="206"/>
+      <c r="J3" s="206"/>
+      <c r="K3" s="206"/>
+      <c r="L3" s="206"/>
+      <c r="M3" s="206"/>
+      <c r="N3" s="206"/>
+      <c r="O3" s="206"/>
+      <c r="P3" s="206"/>
+      <c r="Q3" s="206"/>
+      <c r="R3" s="206"/>
+      <c r="S3" s="206"/>
+      <c r="T3" s="206"/>
+      <c r="U3" s="206"/>
+      <c r="V3" s="206"/>
+      <c r="W3" s="206"/>
+      <c r="X3" s="206"/>
+      <c r="Y3" s="206"/>
+      <c r="Z3" s="206"/>
+      <c r="AA3" s="206"/>
       <c r="AB3" s="162"/>
     </row>
-    <row r="4" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="206" t="s">
+      <c r="B4" s="218" t="s">
         <v>113</v>
       </c>
-      <c r="C4" s="207"/>
-      <c r="D4" s="207"/>
-      <c r="E4" s="207"/>
-      <c r="F4" s="207"/>
-      <c r="G4" s="208"/>
+      <c r="C4" s="219"/>
+      <c r="D4" s="219"/>
+      <c r="E4" s="219"/>
+      <c r="F4" s="219"/>
+      <c r="G4" s="220"/>
       <c r="H4" s="74"/>
-      <c r="I4" s="215" t="s">
+      <c r="I4" s="209" t="s">
         <v>114</v>
       </c>
-      <c r="J4" s="215"/>
-      <c r="K4" s="215"/>
-      <c r="L4" s="215"/>
-      <c r="M4" s="215"/>
-      <c r="N4" s="215"/>
+      <c r="J4" s="209"/>
+      <c r="K4" s="209"/>
+      <c r="L4" s="209"/>
+      <c r="M4" s="209"/>
+      <c r="N4" s="209"/>
       <c r="O4" s="132"/>
-      <c r="P4" s="221" t="s">
+      <c r="P4" s="215" t="s">
         <v>115</v>
       </c>
-      <c r="Q4" s="215"/>
-      <c r="R4" s="215"/>
-      <c r="S4" s="215"/>
-      <c r="T4" s="215"/>
-      <c r="U4" s="222"/>
+      <c r="Q4" s="209"/>
+      <c r="R4" s="209"/>
+      <c r="S4" s="209"/>
+      <c r="T4" s="209"/>
+      <c r="U4" s="216"/>
       <c r="V4" s="132"/>
-      <c r="W4" s="218" t="s">
+      <c r="W4" s="212" t="s">
         <v>116</v>
       </c>
-      <c r="X4" s="219"/>
-      <c r="Y4" s="219"/>
-      <c r="Z4" s="219"/>
-      <c r="AA4" s="219"/>
-      <c r="AB4" s="220"/>
-    </row>
-    <row r="5" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="X4" s="213"/>
+      <c r="Y4" s="213"/>
+      <c r="Z4" s="213"/>
+      <c r="AA4" s="213"/>
+      <c r="AB4" s="214"/>
+    </row>
+    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="209" t="s">
+      <c r="B5" s="221" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="210"/>
-      <c r="D5" s="210" t="s">
+      <c r="C5" s="222"/>
+      <c r="D5" s="222" t="s">
         <v>121</v>
       </c>
-      <c r="E5" s="210"/>
-      <c r="F5" s="210" t="s">
+      <c r="E5" s="222"/>
+      <c r="F5" s="222" t="s">
         <v>122</v>
       </c>
-      <c r="G5" s="211"/>
+      <c r="G5" s="223"/>
       <c r="H5" s="74"/>
       <c r="I5" s="174" t="s">
         <v>81</v>
       </c>
-      <c r="J5" s="213"/>
-      <c r="K5" s="213" t="s">
+      <c r="J5" s="207"/>
+      <c r="K5" s="207" t="s">
         <v>98</v>
       </c>
-      <c r="L5" s="213"/>
-      <c r="M5" s="213" t="s">
+      <c r="L5" s="207"/>
+      <c r="M5" s="207" t="s">
         <v>99</v>
       </c>
-      <c r="N5" s="214"/>
+      <c r="N5" s="208"/>
       <c r="P5" s="146" t="s">
         <v>82</v>
       </c>
@@ -5359,20 +5858,20 @@
         <v>101</v>
       </c>
       <c r="U5" s="148"/>
-      <c r="W5" s="223" t="s">
+      <c r="W5" s="217" t="s">
         <v>117</v>
       </c>
-      <c r="X5" s="216"/>
-      <c r="Y5" s="216" t="s">
+      <c r="X5" s="210"/>
+      <c r="Y5" s="210" t="s">
         <v>118</v>
       </c>
-      <c r="Z5" s="216"/>
-      <c r="AA5" s="216" t="s">
+      <c r="Z5" s="210"/>
+      <c r="AA5" s="210" t="s">
         <v>119</v>
       </c>
-      <c r="AB5" s="217"/>
-    </row>
-    <row r="6" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AB5" s="211"/>
+    </row>
+    <row r="6" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -5452,15 +5951,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="B3:AB3"/>
     <mergeCell ref="I5:J5"/>
@@ -5474,6 +5969,10 @@
     <mergeCell ref="T5:U5"/>
     <mergeCell ref="P4:U4"/>
     <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>